<commit_message>
updated development note SNP counts files
</commit_message>
<xml_diff>
--- a/development_notes/development_run_results.xlsx
+++ b/development_notes/development_run_results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20357"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brandon\Documents\ISSRseq\development notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Otterbein\Desktop\ISSRseq dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8CD8505-E08D-48C6-850D-146D4CEA0E0A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D772C31D-70E7-493A-914B-6782E9C09FD6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="105" yWindow="990" windowWidth="24780" windowHeight="11835" xr2:uid="{99C3184B-795E-4B96-8633-BF33F0E94C1E}"/>
   </bookViews>
@@ -20,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="31">
   <si>
     <t>Taxon</t>
   </si>
@@ -118,6 +112,12 @@
   </si>
   <si>
     <t>variants</t>
+  </si>
+  <si>
+    <t>Corallorhiza bentleyi -ginger dev</t>
+  </si>
+  <si>
+    <t>3,185 (250 bp min)</t>
   </si>
 </sst>
 </file>
@@ -141,12 +141,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -161,7 +167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -173,6 +179,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -489,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4DFE0D0-A0D4-41B8-9114-A09382CB63CC}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,41 +624,41 @@
         <v>174</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="4" t="s">
+    <row r="4" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="2">
-        <v>1075811</v>
-      </c>
-      <c r="G4" s="2">
-        <v>12095</v>
-      </c>
-      <c r="H4" s="2">
-        <v>8542</v>
-      </c>
-      <c r="I4" s="2">
-        <v>492</v>
-      </c>
-      <c r="J4" s="1">
-        <v>0</v>
+      <c r="E4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="8">
+        <v>1435470</v>
+      </c>
+      <c r="G4" s="8">
+        <v>130540</v>
+      </c>
+      <c r="H4" s="8">
+        <v>40447</v>
+      </c>
+      <c r="I4" s="8">
+        <v>32712</v>
+      </c>
+      <c r="J4" s="8">
+        <v>11942</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>14</v>
@@ -649,86 +667,86 @@
         <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1075811</v>
+      </c>
+      <c r="G5" s="2">
+        <v>12095</v>
+      </c>
+      <c r="H5" s="2">
+        <v>8542</v>
+      </c>
+      <c r="I5" s="2">
+        <v>492</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G6" s="2">
         <v>1440</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H6" s="1">
         <v>632</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="4"/>
-    </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="2">
-        <v>17680</v>
-      </c>
-      <c r="F7" s="2">
-        <v>1542360</v>
-      </c>
-      <c r="G7" s="2">
-        <v>4256</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="B7" s="4"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="E8" s="2">
+        <v>17680</v>
       </c>
       <c r="F8" s="2">
-        <v>979456</v>
+        <v>1542360</v>
       </c>
       <c r="G8" s="2">
-        <v>3644</v>
-      </c>
-      <c r="H8" s="2">
-        <v>1430</v>
-      </c>
-      <c r="I8" s="2">
-        <v>885</v>
-      </c>
-      <c r="J8" s="1">
-        <v>648</v>
+        <v>4256</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -736,24 +754,56 @@
         <v>12</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="2">
+        <v>979456</v>
+      </c>
+      <c r="G9" s="2">
+        <v>3644</v>
+      </c>
+      <c r="H9" s="2">
+        <v>1430</v>
+      </c>
+      <c r="I9" s="2">
+        <v>885</v>
+      </c>
+      <c r="J9" s="1">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E10" s="2">
         <v>3852</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G10" s="1">
         <v>209</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>